<commit_message>
Agregar prioridad y ocupacion
</commit_message>
<xml_diff>
--- a/Output/LPM/etapa1_output.xlsx
+++ b/Output/LPM/etapa1_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,86 +481,102 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
+          <t>Prioridad</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
           <t>Avg Fichas</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Std Fichas</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Avg Cirug</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Std Cirug</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Avg Ratio</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Std Ratio</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Ocupación</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>vCp0s8d11</t>
+          <t>vAp0n200s12d1</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>13416.46</v>
+        <v>8312.780000000001</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Fact</t>
+          <t>Opt</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>205220</v>
+        <v>59000</v>
       </c>
       <c r="E2" t="n">
-        <v>391719.53</v>
+        <v>59000</v>
       </c>
       <c r="F2" t="n">
-        <v>0.91</v>
+        <v>0</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>342.72</t>
+          <t>25.26</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>1808.61</v>
+        <v>12.98</v>
       </c>
       <c r="I2" t="n">
-        <v>211</v>
+        <v>55</v>
       </c>
       <c r="J2" t="n">
-        <v>253.1</v>
+        <v>55</v>
       </c>
       <c r="K2" t="n">
-        <v>145.3</v>
+        <v>53.2</v>
       </c>
       <c r="L2" t="n">
-        <v>26.4</v>
+        <v>37.7</v>
       </c>
       <c r="M2" t="n">
-        <v>14.7</v>
+        <v>5.5</v>
       </c>
       <c r="N2" t="n">
-        <v>9.199999999999999</v>
+        <v>3.5</v>
       </c>
       <c r="O2" t="n">
-        <v>3</v>
+        <v>9.300000000000001</v>
+      </c>
+      <c r="P2" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>